<commit_message>
Added support for photoresistor
</commit_message>
<xml_diff>
--- a/Project/TouchGFX/assets/texts/texts.xlsx
+++ b/Project/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1704" uniqueCount="85">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -240,6 +240,36 @@
   </si>
   <si>
     <t xml:space="preserve">New Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Light:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MQTT Messages:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId27</t>
   </si>
 </sst>
 </file>
@@ -1483,7 +1513,9 @@
       </c>
       <c r="G4"/>
       <c r="H4"/>
-      <c r="I4"/>
+      <c r="I4" t="s">
+        <v>78</v>
+      </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
         <v>9</v>
@@ -1736,7 +1768,7 @@
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
@@ -1748,29 +1780,29 @@
         <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
         <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
@@ -1782,12 +1814,12 @@
         <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
@@ -1804,7 +1836,7 @@
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
@@ -1816,12 +1848,12 @@
         <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
@@ -1833,29 +1865,29 @@
         <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
         <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
@@ -1867,12 +1899,12 @@
         <v>44</v>
       </c>
       <c r="F13" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
@@ -1884,29 +1916,29 @@
         <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
         <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
@@ -1918,12 +1950,12 @@
         <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
@@ -1935,12 +1967,12 @@
         <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
@@ -1952,12 +1984,12 @@
         <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
@@ -1969,10 +2001,43 @@
         <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added support for Dallas DS18B20 temperature sensor connected via 1-wire interface
</commit_message>
<xml_diff>
--- a/Project/TouchGFX/assets/texts/texts.xlsx
+++ b/Project/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1704" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="87">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -270,6 +270,12 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;°C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.,</t>
   </si>
 </sst>
 </file>
@@ -1511,7 +1517,9 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4"/>
+      <c r="G4" t="s">
+        <v>86</v>
+      </c>
       <c r="H4"/>
       <c r="I4" t="s">
         <v>78</v>
@@ -2001,7 +2009,7 @@
         <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20">

</xml_diff>

<commit_message>
Added support for MQTT messages from MQTT broker, changed main screen
</commit_message>
<xml_diff>
--- a/Project/TouchGFX/assets/texts/texts.xlsx
+++ b/Project/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3015" uniqueCount="94">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -276,6 +276,27 @@
   </si>
   <si>
     <t xml:space="preserve">.,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.,,0-255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,a-z,A-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!@#$%^&amp;*()_+-=,.&lt;&gt;;':"[]{}\|`~</t>
   </si>
 </sst>
 </file>
@@ -1518,11 +1539,11 @@
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="H4"/>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
@@ -2046,6 +2067,24 @@
         <v>83</v>
       </c>
     </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added code for ESP32, added sending measured values to broker from LightScreen and TempScreen pages
</commit_message>
<xml_diff>
--- a/Project/TouchGFX/assets/texts/texts.xlsx
+++ b/Project/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3015" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3145" uniqueCount="94">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2024,7 +2024,7 @@
         <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E19" t="s">
         <v>44</v>

</xml_diff>